<commit_message>
Moved files to test base and refined test cases and pages
</commit_message>
<xml_diff>
--- a/testData/Data.xlsx
+++ b/testData/Data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dular\OneDrive\Documents\IntelliJ\OpenCartTesting\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B29DD71-EB48-4DF7-8D0D-BAF5D4DE5B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C97E3F9-DB1C-4748-9C5A-DE2C6BA716F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Forgot Password" sheetId="3" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Register" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Username</t>
   </si>
@@ -36,18 +38,6 @@
     <t>jhon123</t>
   </si>
   <si>
-    <t>doe123</t>
-  </si>
-  <si>
-    <t>kali</t>
-  </si>
-  <si>
-    <t>mint123</t>
-  </si>
-  <si>
-    <t>aisu123@</t>
-  </si>
-  <si>
     <t>dulara@demo.com</t>
   </si>
   <si>
@@ -57,56 +47,60 @@
     <t>jhon@demo.site</t>
   </si>
   <si>
-    <t>doe@demo.site</t>
-  </si>
-  <si>
-    <t>mint@demo.site</t>
-  </si>
-  <si>
-    <t>kali@demo.site</t>
-  </si>
-  <si>
-    <t>aisu@demo.site</t>
-  </si>
-  <si>
-    <t>jhondoe123@demo.site</t>
-  </si>
-  <si>
-    <t>jhon1234</t>
-  </si>
-  <si>
-    <t>alex@demo.site</t>
-  </si>
-  <si>
-    <t>alex1234</t>
-  </si>
-  <si>
-    <t>mike@demo.site</t>
-  </si>
-  <si>
-    <t>mike1234</t>
-  </si>
-  <si>
-    <t>salman@demo.site</t>
-  </si>
-  <si>
-    <t>Salma@1234</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Dulara</t>
+  </si>
+  <si>
+    <t>weerakoon</t>
+  </si>
+  <si>
+    <t>dulara1234</t>
+  </si>
+  <si>
+    <t>jhon12345@demo.site</t>
+  </si>
+  <si>
+    <t>Aishan</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>aishan@demo.com</t>
+  </si>
+  <si>
+    <t>aishan1234</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -122,10 +116,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.3"/>
-      <color rgb="FF6AAB73"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,13 +142,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -436,122 +431,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692DB763-AF98-4B0B-9EC0-D56E3B6D08BB}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F2057AE3-AAE4-40F4-B9C4-40F3AEA70AA1}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{5341E89F-7848-435B-950B-45113E6E3667}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F1632D-27DD-4621-A0E4-6769421328B2}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7E54F351-D80A-4DAB-985D-A4888C6D2D22}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3111C713-604F-4867-B80E-3C052A55346D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3414FFDE-FDB3-4390-B0FB-8F5D0BBA61F8}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{7E6BF6ED-A734-440D-9CE6-5484F0FCD33D}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{575F89B2-A43C-4A69-BFC4-5E6585260B90}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{CCF7871B-8197-4D7D-8B6E-D0F84D913F22}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{0E876F5F-9F48-4D47-9FFA-C1F3866A9585}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{2C28CEDA-6191-46C7-A0AF-25287CE675B5}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{A9945468-C61B-44F2-9E8F-C2A4C93FF69C}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{A3FAF100-3123-48B9-9318-AF924304D18C}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{8088AC76-C297-4411-BFDE-912A11B5C98F}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{B13E7105-D0FB-4B66-BD7B-82009505F5F0}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{C0D5A9E3-3C93-4C1D-A041-71FD05663836}"/>
-    <hyperlink ref="B11" r:id="rId11" xr:uid="{67A64131-6005-45AF-A06F-03889203081D}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{68DAB970-2753-41BC-B9EC-2A93E00CE075}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1CCFAD72-3B54-4324-A315-1CABC17D0593}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>